<commit_message>
Formatting Use Case Description
</commit_message>
<xml_diff>
--- a/INTEXUseCases.xlsx
+++ b/INTEXUseCases.xlsx
@@ -567,23 +567,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,117 +618,9 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -837,6 +729,60 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1093,6 +1039,60 @@
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1114,11 +1114,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla8" displayName="Tabla8" ref="B4:C16" totalsRowShown="0" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla8" displayName="Tabla8" ref="B4:C16" totalsRowShown="0" dataDxfId="27">
   <autoFilter ref="B4:C16"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Use Case" dataDxfId="1"/>
-    <tableColumn id="2" name="Users/actors" dataDxfId="0"/>
+    <tableColumn id="1" name="Use Case" dataDxfId="26"/>
+    <tableColumn id="2" name="Users/actors" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium27" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1128,8 +1128,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla18345" displayName="Tabla18345" ref="B99:C118" totalsRowShown="0">
   <autoFilter ref="B99:C118"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Use Case" dataDxfId="9"/>
-    <tableColumn id="2" name="Users/actors" dataDxfId="8"/>
+    <tableColumn id="1" name="Use Case" dataDxfId="3"/>
+    <tableColumn id="2" name="Users/actors" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium27" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1139,27 +1139,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla183456" displayName="Tabla183456" ref="B121:C132" totalsRowShown="0">
   <autoFilter ref="B121:C132"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Use Case" dataDxfId="4"/>
-    <tableColumn id="2" name="Users/actors" dataDxfId="3"/>
+    <tableColumn id="1" name="Use Case" dataDxfId="1"/>
+    <tableColumn id="2" name="Users/actors" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium27" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla13" displayName="Tabla13" ref="B27:C41" totalsRowShown="0" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla13" displayName="Tabla13" ref="B27:C41" totalsRowShown="0" dataDxfId="24">
   <autoFilter ref="B27:C41"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Use Case" dataDxfId="26"/>
-    <tableColumn id="2" name="Users/actors" dataDxfId="25"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium27" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabla14" displayName="Tabla14" ref="B44:C49" totalsRowShown="0" dataDxfId="24">
-  <autoFilter ref="B44:C49"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Use Case" dataDxfId="23"/>
     <tableColumn id="2" name="Users/actors" dataDxfId="22"/>
@@ -1168,9 +1157,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabla16" displayName="Tabla16" ref="B54:C64" totalsRowShown="0" dataDxfId="21">
-  <autoFilter ref="B54:C64"/>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabla14" displayName="Tabla14" ref="B44:C49" totalsRowShown="0" dataDxfId="21">
+  <autoFilter ref="B44:C49"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Use Case" dataDxfId="20"/>
     <tableColumn id="2" name="Users/actors" dataDxfId="19"/>
@@ -1179,12 +1168,23 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tabla17" displayName="Tabla17" ref="B67:C73" totalsRowShown="0" dataDxfId="18">
-  <autoFilter ref="B67:C73"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabla16" displayName="Tabla16" ref="B54:C64" totalsRowShown="0" dataDxfId="18">
+  <autoFilter ref="B54:C64"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Use Case" dataDxfId="17"/>
     <tableColumn id="2" name="Users/actors" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium27" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tabla17" displayName="Tabla17" ref="B67:C73" totalsRowShown="0" dataDxfId="15">
+  <autoFilter ref="B67:C73"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Use Case" dataDxfId="14"/>
+    <tableColumn id="2" name="Users/actors" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium27" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1194,19 +1194,19 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tabla18" displayName="Tabla18" ref="B76:C80" totalsRowShown="0">
   <autoFilter ref="B76:C80"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Use Case" dataDxfId="15"/>
-    <tableColumn id="2" name="Users/actors" dataDxfId="14"/>
+    <tableColumn id="1" name="Use Case" dataDxfId="12"/>
+    <tableColumn id="2" name="Users/actors" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium27" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla82" displayName="Tabla82" ref="B19:C24" totalsRowShown="0" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla82" displayName="Tabla82" ref="B19:C24" totalsRowShown="0" dataDxfId="10">
   <autoFilter ref="B19:C24"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Use Case" dataDxfId="6"/>
-    <tableColumn id="2" name="Users/actors" dataDxfId="5"/>
+    <tableColumn id="1" name="Use Case" dataDxfId="9"/>
+    <tableColumn id="2" name="Users/actors" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium27" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1216,8 +1216,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla183" displayName="Tabla183" ref="B83:C87" totalsRowShown="0">
   <autoFilter ref="B83:C87"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Use Case" dataDxfId="13"/>
-    <tableColumn id="2" name="Users/actors" dataDxfId="12"/>
+    <tableColumn id="1" name="Use Case" dataDxfId="7"/>
+    <tableColumn id="2" name="Users/actors" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium27" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1227,8 +1227,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla1834" displayName="Tabla1834" ref="B90:C96" totalsRowShown="0">
   <autoFilter ref="B90:C96"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Use Case" dataDxfId="11"/>
-    <tableColumn id="2" name="Users/actors" dataDxfId="10"/>
+    <tableColumn id="1" name="Use Case" dataDxfId="5"/>
+    <tableColumn id="2" name="Users/actors" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium27" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1533,8 +1533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1554,10 +1554,10 @@
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="14"/>
+      <c r="C3" s="18"/>
     </row>
     <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
@@ -1577,7 +1577,7 @@
       <c r="C5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="15" t="s">
         <v>133</v>
       </c>
     </row>
@@ -1613,7 +1613,7 @@
       <c r="C8" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="15" t="s">
         <v>133</v>
       </c>
     </row>
@@ -1710,10 +1710,10 @@
       <c r="C17" s="9"/>
     </row>
     <row r="18" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="14"/>
+      <c r="C18" s="18"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
@@ -1777,7 +1777,7 @@
       <c r="C24" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="E24" s="15" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1789,10 +1789,10 @@
     </row>
     <row r="26" spans="1:5" s="6" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="14"/>
+      <c r="C26" s="18"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
@@ -1819,13 +1819,13 @@
       <c r="A29" s="11">
         <v>19</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="C29" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E29" s="15" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1839,7 +1839,7 @@
       <c r="C30" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="E30" s="15" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1853,7 +1853,7 @@
       <c r="C31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="E31" s="15" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1901,7 +1901,7 @@
       <c r="C35" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="E35" s="15" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1915,7 +1915,7 @@
       <c r="C36" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E36" s="20" t="s">
+      <c r="E36" s="15" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1941,7 +1941,7 @@
       <c r="C38" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="E38" s="15" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1966,7 +1966,7 @@
       <c r="C40" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E40" s="20" t="s">
+      <c r="E40" s="15" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1980,7 +1980,7 @@
       <c r="C41" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="E41" s="15" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1989,10 +1989,10 @@
       <c r="C42" s="9"/>
     </row>
     <row r="43" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="17"/>
+      <c r="C43" s="19"/>
     </row>
     <row r="44" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B44" s="3" t="s">
@@ -2056,21 +2056,21 @@
       <c r="C49" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E49" s="20" t="s">
+      <c r="E49" s="15" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B50" s="15"/>
-      <c r="C50" s="16"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="21"/>
     </row>
     <row r="51" spans="1:5" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="52" spans="1:5" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="53" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C53" s="17"/>
+      <c r="C53" s="19"/>
     </row>
     <row r="54" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B54" s="3" t="s">
@@ -2195,10 +2195,10 @@
       <c r="C65" s="2"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="13" t="s">
+      <c r="B66" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C66" s="14"/>
+      <c r="C66" s="18"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="3" t="s">
@@ -2279,10 +2279,10 @@
       <c r="C74" s="2"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="13" t="s">
+      <c r="B75" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C75" s="14"/>
+      <c r="C75" s="18"/>
     </row>
     <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="3" t="s">
@@ -2340,10 +2340,10 @@
       <c r="C81" s="1"/>
     </row>
     <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="13" t="s">
+      <c r="B82" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C82" s="14"/>
+      <c r="C82" s="18"/>
     </row>
     <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B83" s="7" t="s">
@@ -2398,10 +2398,10 @@
       </c>
     </row>
     <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="13" t="s">
+      <c r="B89" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="C89" s="14"/>
+      <c r="C89" s="18"/>
     </row>
     <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B90" s="7" t="s">
@@ -2421,7 +2421,7 @@
       <c r="C91" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E91" s="20"/>
+      <c r="E91" s="15"/>
     </row>
     <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="11">
@@ -2444,7 +2444,7 @@
       <c r="C93" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E93" s="20"/>
+      <c r="E93" s="15"/>
     </row>
     <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="11">
@@ -2478,15 +2478,15 @@
       <c r="C96" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="E96" s="20" t="s">
+      <c r="E96" s="15" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="13" t="s">
+      <c r="B98" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="C98" s="14"/>
+      <c r="C98" s="18"/>
     </row>
     <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B99" s="7" t="s">
@@ -2594,7 +2594,7 @@
       <c r="C108" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E108" s="20" t="s">
+      <c r="E108" s="15" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2685,7 +2685,7 @@
       <c r="C116" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E116" s="20" t="s">
+      <c r="E116" s="15" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2712,10 +2712,10 @@
       </c>
     </row>
     <row r="120" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="13" t="s">
+      <c r="B120" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="C120" s="14"/>
+      <c r="C120" s="18"/>
     </row>
     <row r="121" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B121" s="10" t="s">
@@ -2780,7 +2780,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="127" spans="1:5" s="11" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" s="11" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="11">
         <v>91</v>
       </c>
@@ -2790,7 +2790,7 @@
       <c r="C127" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E127" s="20" t="s">
+      <c r="E127" s="15" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2817,17 +2817,17 @@
         <v>117</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="11">
         <v>94</v>
       </c>
-      <c r="B130" s="21" t="s">
+      <c r="B130" s="16" t="s">
         <v>131</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E130" s="20" t="s">
+      <c r="E130" s="15" t="s">
         <v>137</v>
       </c>
     </row>

</xml_diff>